<commit_message>
hpo SR with smaller offset
</commit_message>
<xml_diff>
--- a/julia-nix-slurm-env-main/HPOErgebnisse.xlsx
+++ b/julia-nix-slurm-env-main/HPOErgebnisse.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\49160\Documents\Master\Masterarbeit\OC-MasterThesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\49160\Documents\Master\Masterarbeit\OC-MasterThesis\julia-nix-slurm-env-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12088A6-CC76-4E17-B141-6EBD17A5340E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA49422F-F509-46EE-8FFD-7FD2C8A49AA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{FC45CD7E-7F2F-48B4-8C22-E79589995154}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" activeTab="1" xr2:uid="{FC45CD7E-7F2F-48B4-8C22-E79589995154}"/>
   </bookViews>
   <sheets>
     <sheet name="Parity" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="25">
   <si>
     <t>Konstant</t>
   </si>
@@ -104,13 +104,24 @@
   <si>
     <t>Mittelwert:</t>
   </si>
+  <si>
+    <t>Notizen</t>
+  </si>
+  <si>
+    <t>Bester Wert hat kein Offset! Zweitbesten nehmen! Werte Bester: [1800, 58, 0.5, 20, 0]</t>
+  </si>
+  <si>
+    <t>Bester Wert hat kein Offset! Zweitbesten nehmen! Werte Bester: [1000, 44, 0.015, 12, 0]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.00000000"/>
+    <numFmt numFmtId="179" formatCode="0.00000000"/>
+    <numFmt numFmtId="180" formatCode="0.000000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -276,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -298,11 +309,41 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="179" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="179" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="31">
+  <dxfs count="32">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -981,39 +1022,40 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{98A828E8-F85F-42E5-A901-CC423FF08826}" name="Tabelle1" displayName="Tabelle1" ref="A1:J20" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
-  <autoFilter ref="A1:J20" xr:uid="{98A828E8-F85F-42E5-A901-CC423FF08826}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{F50F2258-E4C2-44D3-B197-D549748B1AA6}" name="Rekombinationstyp" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{4EAA17DC-ECCB-42FE-87FB-B37443776E06}" name="Typ Rekombinationsrate" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{041E9CBC-7CE4-48BB-A7AA-7F30F7569802}" name="mit / ohne Offset" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{7E07C587-1EB0-46B8-8F3E-3E35F9D0164D}" name="Anzahl Rechenknoten" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{D4DEF5B0-A627-47E8-8759-112E0628B432}" name="Populationsgröße" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{33BA195D-8889-4763-870A-82A2CAD42ED1}" name="(Start-) Rekombinationsrate" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{D42B36FD-F1B8-4765-B14B-0AB4CD534307}" name="Delta Rekombinationsrate" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{BF2EEC5F-7304-428F-BD91-0C65B3BEE72F}" name="Anzahl Elitisten" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{5570D174-D9C8-401C-BF23-66D36038F518}" name="Offset" dataDxfId="17"/>
-    <tableColumn id="10" xr3:uid="{53F23BD6-14B8-41B8-857A-3A139FD7C9A4}" name="Iterationen" dataDxfId="16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{98A828E8-F85F-42E5-A901-CC423FF08826}" name="Tabelle1" displayName="Tabelle1" ref="A1:K20" totalsRowShown="0" headerRowDxfId="31" dataDxfId="29" headerRowBorderDxfId="30" tableBorderDxfId="28" totalsRowBorderDxfId="27">
+  <autoFilter ref="A1:K20" xr:uid="{98A828E8-F85F-42E5-A901-CC423FF08826}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{F50F2258-E4C2-44D3-B197-D549748B1AA6}" name="Rekombinationstyp" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{4EAA17DC-ECCB-42FE-87FB-B37443776E06}" name="Typ Rekombinationsrate" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{041E9CBC-7CE4-48BB-A7AA-7F30F7569802}" name="mit / ohne Offset" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{7E07C587-1EB0-46B8-8F3E-3E35F9D0164D}" name="Anzahl Rechenknoten" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{D4DEF5B0-A627-47E8-8759-112E0628B432}" name="Populationsgröße" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{33BA195D-8889-4763-870A-82A2CAD42ED1}" name="(Start-) Rekombinationsrate" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{D42B36FD-F1B8-4765-B14B-0AB4CD534307}" name="Delta Rekombinationsrate" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{BF2EEC5F-7304-428F-BD91-0C65B3BEE72F}" name="Anzahl Elitisten" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{5570D174-D9C8-401C-BF23-66D36038F518}" name="Offset" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{53F23BD6-14B8-41B8-857A-3A139FD7C9A4}" name="Iterationen" dataDxfId="17"/>
+    <tableColumn id="11" xr3:uid="{16F8028F-1019-46E3-A47D-C03426554D87}" name="Notizen" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3262786E-EADB-4970-8DCB-0C3E2CA0491F}" name="Tabelle13" displayName="Tabelle13" ref="A1:K21" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3262786E-EADB-4970-8DCB-0C3E2CA0491F}" name="Tabelle13" displayName="Tabelle13" ref="A1:K21" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" totalsRowBorderDxfId="12">
   <autoFilter ref="A1:K21" xr:uid="{3262786E-EADB-4970-8DCB-0C3E2CA0491F}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{EBC23620-6299-4F9E-A03B-152D8E926588}" name="Rekombinationstyp" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{CE58E6EA-5E62-4C09-A41A-25E14FAF4683}" name="Typ Rekombinationsrate" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{BA2EBEAD-E4F6-4987-A4E4-1071392DCCA5}" name="mit / ohne Offset" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{D80D805A-F3FB-480D-B4C5-4B4895EEB25F}" name="Anzahl Rechenknoten" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{A9B0E371-630B-42B8-8C42-C5655A4B7427}" name="Populationsgröße" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{7D465FE8-FC65-4466-9518-38A3A9D9BCF4}" name="(Start-) Rekombinationsrate" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{4E443DEE-E707-4BA3-B361-077E8DABF672}" name="Delta Rekombinationsrate" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{DE16DA46-B7E3-4CA6-BD65-AD82812E3778}" name="Anzahl Elitisten" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{56ED5AAA-44A8-44EB-A016-F7592A40B9FE}" name="Offset" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{02B02A40-7CC6-460A-9FEA-54286618D688}" name="Iterationen" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{44D1ABA5-7523-42BC-8FF9-CC1C035DB5D4}" name="Fitness" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{EBC23620-6299-4F9E-A03B-152D8E926588}" name="Rekombinationstyp" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{CE58E6EA-5E62-4C09-A41A-25E14FAF4683}" name="Typ Rekombinationsrate" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{BA2EBEAD-E4F6-4987-A4E4-1071392DCCA5}" name="mit / ohne Offset" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{D80D805A-F3FB-480D-B4C5-4B4895EEB25F}" name="Anzahl Rechenknoten" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{A9B0E371-630B-42B8-8C42-C5655A4B7427}" name="Populationsgröße" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{7D465FE8-FC65-4466-9518-38A3A9D9BCF4}" name="(Start-) Rekombinationsrate" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{4E443DEE-E707-4BA3-B361-077E8DABF672}" name="Delta Rekombinationsrate" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{DE16DA46-B7E3-4CA6-BD65-AD82812E3778}" name="Anzahl Elitisten" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{56ED5AAA-44A8-44EB-A016-F7592A40B9FE}" name="Offset" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{02B02A40-7CC6-460A-9FEA-54286618D688}" name="Iterationen" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{44D1ABA5-7523-42BC-8FF9-CC1C035DB5D4}" name="Fitness" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1336,10 +1378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24624115-2EA4-43F4-B7C3-9E45AC575B2C}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView topLeftCell="F4" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1353,10 +1395,11 @@
     <col min="7" max="7" width="25.08984375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="71.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1387,8 +1430,11 @@
       <c r="J1" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1419,22 +1465,38 @@
       <c r="J2" s="15">
         <v>74.599998474121094</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K2" s="7"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="6"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D3" s="5">
+        <v>1500</v>
+      </c>
+      <c r="E3" s="5">
+        <v>50</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5">
+        <v>18</v>
+      </c>
+      <c r="I3" s="5">
+        <v>25</v>
+      </c>
+      <c r="J3" s="15">
+        <v>58.799999237060497</v>
+      </c>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="4"/>
       <c r="B4" s="5" t="s">
         <v>4</v>
@@ -1460,25 +1522,41 @@
       <c r="I4" s="5">
         <v>0</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="21">
         <v>71</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="6"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D5" s="5">
+        <v>1600</v>
+      </c>
+      <c r="E5" s="5">
+        <v>58</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="H5" s="5">
+        <v>20</v>
+      </c>
+      <c r="I5" s="5">
+        <v>25</v>
+      </c>
+      <c r="J5" s="15">
+        <v>46.299999237060497</v>
+      </c>
+      <c r="K5" s="5"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="B6" s="5" t="s">
         <v>1</v>
@@ -1504,25 +1582,43 @@
       <c r="I6" s="5">
         <v>0</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="21">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="6"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D7" s="5">
+        <v>1100</v>
+      </c>
+      <c r="E7" s="5">
+        <v>54</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0.35</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0</v>
+      </c>
+      <c r="H7" s="5">
+        <v>20</v>
+      </c>
+      <c r="I7" s="5">
+        <v>30</v>
+      </c>
+      <c r="J7" s="21">
+        <v>57.6</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>6</v>
       </c>
@@ -1550,25 +1646,41 @@
       <c r="I8" s="9">
         <v>0</v>
       </c>
-      <c r="J8" s="10">
+      <c r="J8" s="22">
         <v>55</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="10"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D9" s="9">
+        <v>850</v>
+      </c>
+      <c r="E9" s="9">
+        <v>54</v>
+      </c>
+      <c r="F9" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="G9" s="9">
+        <v>0</v>
+      </c>
+      <c r="H9" s="9">
+        <v>16</v>
+      </c>
+      <c r="I9" s="9">
+        <v>15</v>
+      </c>
+      <c r="J9" s="22">
+        <v>57.599998474121001</v>
+      </c>
+      <c r="K9" s="5"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="8"/>
       <c r="B10" s="9" t="s">
         <v>4</v>
@@ -1597,22 +1709,40 @@
       <c r="J10" s="10">
         <v>44.599998474121001</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="8"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="10"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D11" s="9">
+        <v>1700</v>
+      </c>
+      <c r="E11" s="9">
+        <v>28</v>
+      </c>
+      <c r="F11" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="G11" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="H11" s="9">
+        <v>12</v>
+      </c>
+      <c r="I11" s="9">
+        <v>20</v>
+      </c>
+      <c r="J11" s="22">
+        <v>62.5</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="8"/>
       <c r="B12" s="9" t="s">
         <v>1</v>
@@ -1641,22 +1771,38 @@
       <c r="J12" s="16">
         <v>72.400001525878906</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="8"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="10"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D13" s="9">
+        <v>950</v>
+      </c>
+      <c r="E13" s="9">
+        <v>58</v>
+      </c>
+      <c r="F13" s="9">
+        <v>0.7</v>
+      </c>
+      <c r="G13" s="9">
+        <v>0</v>
+      </c>
+      <c r="H13" s="9">
+        <v>10</v>
+      </c>
+      <c r="I13" s="9">
+        <v>15</v>
+      </c>
+      <c r="J13" s="10">
+        <v>61.099998474121001</v>
+      </c>
+      <c r="K13" s="5"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>7</v>
       </c>
@@ -1687,22 +1833,38 @@
       <c r="J14" s="6">
         <v>35.299999237060497</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K14" s="5"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="6"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D15" s="5">
+        <v>1400</v>
+      </c>
+      <c r="E15" s="5">
+        <v>54</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="G15" s="5">
+        <v>0</v>
+      </c>
+      <c r="H15" s="5">
+        <v>20</v>
+      </c>
+      <c r="I15" s="5">
+        <v>45</v>
+      </c>
+      <c r="J15" s="6">
+        <v>47.599998474121001</v>
+      </c>
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="4"/>
       <c r="B16" s="5" t="s">
         <v>4</v>
@@ -1731,22 +1893,38 @@
       <c r="J16" s="6">
         <v>70.199996948242102</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="6"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D17" s="5">
+        <v>1500</v>
+      </c>
+      <c r="E17" s="5">
+        <v>52</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="G17" s="5">
+        <v>0.04</v>
+      </c>
+      <c r="H17" s="5">
+        <v>18</v>
+      </c>
+      <c r="I17" s="5">
+        <v>25</v>
+      </c>
+      <c r="J17" s="21">
+        <v>46.5</v>
+      </c>
+      <c r="K17" s="5"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
       <c r="B18" s="5" t="s">
         <v>1</v>
@@ -1775,22 +1953,38 @@
       <c r="J18" s="6">
         <v>41.900001525878899</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K18" s="5"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="6"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D19" s="5">
+        <v>250</v>
+      </c>
+      <c r="E19" s="5">
+        <v>50</v>
+      </c>
+      <c r="F19" s="5">
+        <v>0.35</v>
+      </c>
+      <c r="G19" s="5">
+        <v>0</v>
+      </c>
+      <c r="H19" s="5">
+        <v>16</v>
+      </c>
+      <c r="I19" s="5">
+        <v>40</v>
+      </c>
+      <c r="J19" s="6">
+        <v>53.599998474121001</v>
+      </c>
+      <c r="K19" s="5"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
         <v>8</v>
       </c>
@@ -1821,14 +2015,15 @@
       <c r="J20" s="13">
         <v>53.799999237060497</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K20" s="23"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="I22" t="s">
         <v>21</v>
       </c>
       <c r="J22" s="17">
         <f>AVERAGE(Tabelle1[Iterationen])</f>
-        <v>55.179999542236303</v>
+        <v>54.915788831208843</v>
       </c>
     </row>
   </sheetData>
@@ -1843,8 +2038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD7223BD-063A-4B3D-9902-0134A848554C}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="G3" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1907,14 +2102,30 @@
       <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="7"/>
+      <c r="D2" s="5">
+        <v>600</v>
+      </c>
+      <c r="E2" s="5">
+        <v>50</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="G2" s="5">
+        <v>0</v>
+      </c>
+      <c r="H2" s="5">
+        <v>20</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0</v>
+      </c>
+      <c r="J2" s="6">
+        <v>281.3</v>
+      </c>
+      <c r="K2" s="24">
+        <v>1.33039699867367E-2</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
@@ -2133,14 +2344,30 @@
       <c r="C12" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="9"/>
+      <c r="D12" s="9">
+        <v>1350</v>
+      </c>
+      <c r="E12" s="9">
+        <v>40</v>
+      </c>
+      <c r="F12" s="9">
+        <v>0.35</v>
+      </c>
+      <c r="G12" s="9">
+        <v>0</v>
+      </c>
+      <c r="H12" s="9">
+        <v>20</v>
+      </c>
+      <c r="I12" s="9">
+        <v>0</v>
+      </c>
+      <c r="J12" s="10">
+        <v>288.60000000000002</v>
+      </c>
+      <c r="K12" s="25">
+        <v>9.9280597642064095E-3</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="8"/>
@@ -2309,14 +2536,30 @@
       </c>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="12"/>
+      <c r="D20" s="12">
+        <v>1850</v>
+      </c>
+      <c r="E20" s="12">
+        <v>44</v>
+      </c>
+      <c r="F20" s="12">
+        <v>0</v>
+      </c>
+      <c r="G20" s="12">
+        <v>0</v>
+      </c>
+      <c r="H20" s="12">
+        <v>20</v>
+      </c>
+      <c r="I20" s="12">
+        <v>0</v>
+      </c>
+      <c r="J20" s="13">
+        <v>377.4</v>
+      </c>
+      <c r="K20" s="26">
+        <v>1.2776309624314299E-2</v>
+      </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="19"/>
@@ -2332,7 +2575,7 @@
       </c>
       <c r="J21" s="20">
         <f>AVERAGE(J2:J20)</f>
-        <v>323.64285714285717</v>
+        <v>321.27999999999997</v>
       </c>
       <c r="K21" s="18"/>
     </row>

</xml_diff>

<commit_message>
finished encode and started decode
</commit_message>
<xml_diff>
--- a/julia-nix-slurm-env-main/HPOErgebnisse.xlsx
+++ b/julia-nix-slurm-env-main/HPOErgebnisse.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\49160\Documents\Master\Masterarbeit\OC-MasterThesis\julia-nix-slurm-env-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B772EB75-267A-40F7-A2AE-7A0866EC2995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B603C6B-4490-483C-9138-C00E5CF6BF2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" activeTab="1" xr2:uid="{FC45CD7E-7F2F-48B4-8C22-E79589995154}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" activeTab="2" xr2:uid="{FC45CD7E-7F2F-48B4-8C22-E79589995154}"/>
   </bookViews>
   <sheets>
     <sheet name="Parity" sheetId="1" r:id="rId1"/>
     <sheet name="Keijzer" sheetId="2" r:id="rId2"/>
+    <sheet name="Encode" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="27">
   <si>
     <t>Konstant</t>
   </si>
@@ -326,7 +327,283 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
+  <dxfs count="47">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1057,41 +1334,59 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{98A828E8-F85F-42E5-A901-CC423FF08826}" name="Tabelle1" displayName="Tabelle1" ref="A1:K20" totalsRowShown="0" headerRowDxfId="32" dataDxfId="30" headerRowBorderDxfId="31" tableBorderDxfId="29" totalsRowBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{98A828E8-F85F-42E5-A901-CC423FF08826}" name="Tabelle1" displayName="Tabelle1" ref="A1:K20" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
   <autoFilter ref="A1:K20" xr:uid="{98A828E8-F85F-42E5-A901-CC423FF08826}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{F50F2258-E4C2-44D3-B197-D549748B1AA6}" name="Rekombinationstyp" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{4EAA17DC-ECCB-42FE-87FB-B37443776E06}" name="Typ Rekombinationsrate" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{041E9CBC-7CE4-48BB-A7AA-7F30F7569802}" name="mit / ohne Offset" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{7E07C587-1EB0-46B8-8F3E-3E35F9D0164D}" name="Anzahl Rechenknoten" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{D4DEF5B0-A627-47E8-8759-112E0628B432}" name="Populationsgröße" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{33BA195D-8889-4763-870A-82A2CAD42ED1}" name="(Start-) Rekombinationsrate" dataDxfId="22"/>
-    <tableColumn id="7" xr3:uid="{D42B36FD-F1B8-4765-B14B-0AB4CD534307}" name="Delta Rekombinationsrate" dataDxfId="21"/>
-    <tableColumn id="8" xr3:uid="{BF2EEC5F-7304-428F-BD91-0C65B3BEE72F}" name="Anzahl Elitisten" dataDxfId="20"/>
-    <tableColumn id="9" xr3:uid="{5570D174-D9C8-401C-BF23-66D36038F518}" name="Offset" dataDxfId="19"/>
-    <tableColumn id="10" xr3:uid="{53F23BD6-14B8-41B8-857A-3A139FD7C9A4}" name="Iterationen" dataDxfId="18"/>
-    <tableColumn id="11" xr3:uid="{16F8028F-1019-46E3-A47D-C03426554D87}" name="Notizen" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{F50F2258-E4C2-44D3-B197-D549748B1AA6}" name="Rekombinationstyp" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{4EAA17DC-ECCB-42FE-87FB-B37443776E06}" name="Typ Rekombinationsrate" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{041E9CBC-7CE4-48BB-A7AA-7F30F7569802}" name="mit / ohne Offset" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{7E07C587-1EB0-46B8-8F3E-3E35F9D0164D}" name="Anzahl Rechenknoten" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{D4DEF5B0-A627-47E8-8759-112E0628B432}" name="Populationsgröße" dataDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{33BA195D-8889-4763-870A-82A2CAD42ED1}" name="(Start-) Rekombinationsrate" dataDxfId="36"/>
+    <tableColumn id="7" xr3:uid="{D42B36FD-F1B8-4765-B14B-0AB4CD534307}" name="Delta Rekombinationsrate" dataDxfId="35"/>
+    <tableColumn id="8" xr3:uid="{BF2EEC5F-7304-428F-BD91-0C65B3BEE72F}" name="Anzahl Elitisten" dataDxfId="34"/>
+    <tableColumn id="9" xr3:uid="{5570D174-D9C8-401C-BF23-66D36038F518}" name="Offset" dataDxfId="33"/>
+    <tableColumn id="10" xr3:uid="{53F23BD6-14B8-41B8-857A-3A139FD7C9A4}" name="Iterationen" dataDxfId="32"/>
+    <tableColumn id="11" xr3:uid="{16F8028F-1019-46E3-A47D-C03426554D87}" name="Notizen" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3262786E-EADB-4970-8DCB-0C3E2CA0491F}" name="Tabelle13" displayName="Tabelle13" ref="A1:L21" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" totalsRowBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3262786E-EADB-4970-8DCB-0C3E2CA0491F}" name="Tabelle13" displayName="Tabelle13" ref="A1:L21" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <autoFilter ref="A1:L21" xr:uid="{3262786E-EADB-4970-8DCB-0C3E2CA0491F}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{EBC23620-6299-4F9E-A03B-152D8E926588}" name="Rekombinationstyp" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{CE58E6EA-5E62-4C09-A41A-25E14FAF4683}" name="Typ Rekombinationsrate" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{BA2EBEAD-E4F6-4987-A4E4-1071392DCCA5}" name="mit / ohne Offset" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{D80D805A-F3FB-480D-B4C5-4B4895EEB25F}" name="Anzahl Rechenknoten" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{A9B0E371-630B-42B8-8C42-C5655A4B7427}" name="Populationsgröße" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{7D465FE8-FC65-4466-9518-38A3A9D9BCF4}" name="(Start-) Rekombinationsrate" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{4E443DEE-E707-4BA3-B361-077E8DABF672}" name="Delta Rekombinationsrate" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{DE16DA46-B7E3-4CA6-BD65-AD82812E3778}" name="Anzahl Elitisten" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{56ED5AAA-44A8-44EB-A016-F7592A40B9FE}" name="Offset" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{02B02A40-7CC6-460A-9FEA-54286618D688}" name="Iterationen" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{44D1ABA5-7523-42BC-8FF9-CC1C035DB5D4}" name="Fitness" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{8DB525A8-4B8A-476B-970A-75523C0137D6}" name="Notizen" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{EBC23620-6299-4F9E-A03B-152D8E926588}" name="Rekombinationstyp" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{CE58E6EA-5E62-4C09-A41A-25E14FAF4683}" name="Typ Rekombinationsrate" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{BA2EBEAD-E4F6-4987-A4E4-1071392DCCA5}" name="mit / ohne Offset" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{D80D805A-F3FB-480D-B4C5-4B4895EEB25F}" name="Anzahl Rechenknoten" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{A9B0E371-630B-42B8-8C42-C5655A4B7427}" name="Populationsgröße" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{7D465FE8-FC65-4466-9518-38A3A9D9BCF4}" name="(Start-) Rekombinationsrate" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{4E443DEE-E707-4BA3-B361-077E8DABF672}" name="Delta Rekombinationsrate" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{DE16DA46-B7E3-4CA6-BD65-AD82812E3778}" name="Anzahl Elitisten" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{56ED5AAA-44A8-44EB-A016-F7592A40B9FE}" name="Offset" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{02B02A40-7CC6-460A-9FEA-54286618D688}" name="Iterationen" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{44D1ABA5-7523-42BC-8FF9-CC1C035DB5D4}" name="Fitness" dataDxfId="15"/>
+    <tableColumn id="12" xr3:uid="{8DB525A8-4B8A-476B-970A-75523C0137D6}" name="Notizen" dataDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{16E9E3FF-82F7-4D02-89F5-0EFEBB302DBC}" name="Tabelle14" displayName="Tabelle14" ref="A1:I20" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
+  <autoFilter ref="A1:I20" xr:uid="{16E9E3FF-82F7-4D02-89F5-0EFEBB302DBC}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{E3061643-506C-4DF5-9519-25A5F354EE28}" name="Rekombinationstyp" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{1FD88150-3719-40E4-9930-3DAD021E5786}" name="Typ Rekombinationsrate" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{2947C2F6-045E-4DD9-834F-AD1EC2D305C1}" name="mit / ohne Offset" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{D1559373-156A-4445-926B-0BBB80142A0C}" name="Anzahl Rechenknoten" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{B3F81709-CC4C-4398-AAAF-ACC6C4B7DD92}" name="Populationsgröße" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{0455A311-9330-4D66-878D-DE22D808F49F}" name="(Start-) Rekombinationsrate" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{94BA1A90-5769-4BC9-90CB-E9F5241EEC52}" name="Delta Rekombinationsrate" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{6866B354-ACD0-490F-96F7-E4A2DEFB0D0F}" name="Anzahl Elitisten" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{514CBF92-64C9-4012-B295-3CB710414703}" name="Offset" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1416,8 +1711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24624115-2EA4-43F4-B7C3-9E45AC575B2C}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView topLeftCell="I4" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2074,8 +2369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD7223BD-063A-4B3D-9902-0134A848554C}">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2793,4 +3088,516 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23A0EA66-8E87-4152-A235-1FC7EB76D9FD}">
+  <dimension ref="A1:J22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F5" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="71.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="7">
+        <v>4000</v>
+      </c>
+      <c r="E2" s="7">
+        <v>50</v>
+      </c>
+      <c r="F2" s="14"/>
+      <c r="G2" s="7">
+        <v>0</v>
+      </c>
+      <c r="H2" s="7">
+        <v>2</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="7">
+        <v>4000</v>
+      </c>
+      <c r="E3" s="5">
+        <v>50</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5">
+        <v>2</v>
+      </c>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="7">
+        <v>4000</v>
+      </c>
+      <c r="E4" s="5">
+        <v>50</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5">
+        <v>2</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="7">
+        <v>4000</v>
+      </c>
+      <c r="E5" s="5">
+        <v>50</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5">
+        <v>2</v>
+      </c>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="7">
+        <v>4000</v>
+      </c>
+      <c r="E6" s="5">
+        <v>50</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5">
+        <v>0</v>
+      </c>
+      <c r="H6" s="5">
+        <v>2</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="7">
+        <v>4000</v>
+      </c>
+      <c r="E7" s="5">
+        <v>50</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5">
+        <v>0</v>
+      </c>
+      <c r="H7" s="5">
+        <v>2</v>
+      </c>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="9">
+        <v>1500</v>
+      </c>
+      <c r="E8" s="9">
+        <v>44</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9">
+        <v>0</v>
+      </c>
+      <c r="H8" s="9">
+        <v>2</v>
+      </c>
+      <c r="I8" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="9">
+        <v>1500</v>
+      </c>
+      <c r="E9" s="9">
+        <v>44</v>
+      </c>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9">
+        <v>0</v>
+      </c>
+      <c r="H9" s="9">
+        <v>2</v>
+      </c>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="9">
+        <v>1500</v>
+      </c>
+      <c r="E10" s="9">
+        <v>44</v>
+      </c>
+      <c r="F10" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9">
+        <v>2</v>
+      </c>
+      <c r="I10" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="9">
+        <v>1500</v>
+      </c>
+      <c r="E11" s="9">
+        <v>44</v>
+      </c>
+      <c r="F11" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9">
+        <v>2</v>
+      </c>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="9">
+        <v>1500</v>
+      </c>
+      <c r="E12" s="9">
+        <v>44</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9">
+        <v>0</v>
+      </c>
+      <c r="H12" s="9">
+        <v>2</v>
+      </c>
+      <c r="I12" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="8"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="9">
+        <v>1500</v>
+      </c>
+      <c r="E13" s="9">
+        <v>44</v>
+      </c>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9">
+        <v>0</v>
+      </c>
+      <c r="H13" s="9">
+        <v>2</v>
+      </c>
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="5">
+        <v>6500</v>
+      </c>
+      <c r="E14" s="5">
+        <v>40</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5">
+        <v>0</v>
+      </c>
+      <c r="H14" s="9">
+        <v>2</v>
+      </c>
+      <c r="I14" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="5">
+        <v>6500</v>
+      </c>
+      <c r="E15" s="5">
+        <v>40</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5">
+        <v>0</v>
+      </c>
+      <c r="H15" s="9">
+        <v>2</v>
+      </c>
+      <c r="I15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="5">
+        <v>6500</v>
+      </c>
+      <c r="E16" s="5">
+        <v>40</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="9">
+        <v>2</v>
+      </c>
+      <c r="I16" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="5">
+        <v>6500</v>
+      </c>
+      <c r="E17" s="5">
+        <v>40</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="G17" s="5"/>
+      <c r="H17" s="9">
+        <v>2</v>
+      </c>
+      <c r="I17" s="5"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" s="4"/>
+      <c r="B18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="5">
+        <v>6500</v>
+      </c>
+      <c r="E18" s="5">
+        <v>40</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5">
+        <v>0</v>
+      </c>
+      <c r="H18" s="9">
+        <v>2</v>
+      </c>
+      <c r="I18" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="5">
+        <v>6500</v>
+      </c>
+      <c r="E19" s="5">
+        <v>40</v>
+      </c>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5">
+        <v>0</v>
+      </c>
+      <c r="H19" s="9">
+        <v>2</v>
+      </c>
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="12">
+        <v>3000</v>
+      </c>
+      <c r="E20" s="12">
+        <v>50</v>
+      </c>
+      <c r="F20" s="12">
+        <v>0</v>
+      </c>
+      <c r="G20" s="12">
+        <v>0</v>
+      </c>
+      <c r="H20" s="12">
+        <v>2</v>
+      </c>
+      <c r="I20" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J22" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added decode and fixed encode
</commit_message>
<xml_diff>
--- a/julia-nix-slurm-env-main/HPOErgebnisse.xlsx
+++ b/julia-nix-slurm-env-main/HPOErgebnisse.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\49160\Documents\Master\Masterarbeit\OC-MasterThesis\julia-nix-slurm-env-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B603C6B-4490-483C-9138-C00E5CF6BF2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5161894D-FAB0-4FE7-AE65-15E7E408EC74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" activeTab="2" xr2:uid="{FC45CD7E-7F2F-48B4-8C22-E79589995154}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" activeTab="3" xr2:uid="{FC45CD7E-7F2F-48B4-8C22-E79589995154}"/>
   </bookViews>
   <sheets>
     <sheet name="Parity" sheetId="1" r:id="rId1"/>
     <sheet name="Keijzer" sheetId="2" r:id="rId2"/>
     <sheet name="Encode" sheetId="3" r:id="rId3"/>
+    <sheet name="Decode" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="27">
   <si>
     <t>Konstant</t>
   </si>
@@ -327,7 +328,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="47">
+  <dxfs count="61">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -579,6 +580,282 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -1334,59 +1611,77 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{98A828E8-F85F-42E5-A901-CC423FF08826}" name="Tabelle1" displayName="Tabelle1" ref="A1:K20" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{98A828E8-F85F-42E5-A901-CC423FF08826}" name="Tabelle1" displayName="Tabelle1" ref="A1:K20" totalsRowShown="0" headerRowDxfId="60" dataDxfId="58" headerRowBorderDxfId="59" tableBorderDxfId="57" totalsRowBorderDxfId="56">
   <autoFilter ref="A1:K20" xr:uid="{98A828E8-F85F-42E5-A901-CC423FF08826}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{F50F2258-E4C2-44D3-B197-D549748B1AA6}" name="Rekombinationstyp" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{4EAA17DC-ECCB-42FE-87FB-B37443776E06}" name="Typ Rekombinationsrate" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{041E9CBC-7CE4-48BB-A7AA-7F30F7569802}" name="mit / ohne Offset" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{7E07C587-1EB0-46B8-8F3E-3E35F9D0164D}" name="Anzahl Rechenknoten" dataDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{D4DEF5B0-A627-47E8-8759-112E0628B432}" name="Populationsgröße" dataDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{33BA195D-8889-4763-870A-82A2CAD42ED1}" name="(Start-) Rekombinationsrate" dataDxfId="36"/>
-    <tableColumn id="7" xr3:uid="{D42B36FD-F1B8-4765-B14B-0AB4CD534307}" name="Delta Rekombinationsrate" dataDxfId="35"/>
-    <tableColumn id="8" xr3:uid="{BF2EEC5F-7304-428F-BD91-0C65B3BEE72F}" name="Anzahl Elitisten" dataDxfId="34"/>
-    <tableColumn id="9" xr3:uid="{5570D174-D9C8-401C-BF23-66D36038F518}" name="Offset" dataDxfId="33"/>
-    <tableColumn id="10" xr3:uid="{53F23BD6-14B8-41B8-857A-3A139FD7C9A4}" name="Iterationen" dataDxfId="32"/>
-    <tableColumn id="11" xr3:uid="{16F8028F-1019-46E3-A47D-C03426554D87}" name="Notizen" dataDxfId="31"/>
+    <tableColumn id="1" xr3:uid="{F50F2258-E4C2-44D3-B197-D549748B1AA6}" name="Rekombinationstyp" dataDxfId="55"/>
+    <tableColumn id="2" xr3:uid="{4EAA17DC-ECCB-42FE-87FB-B37443776E06}" name="Typ Rekombinationsrate" dataDxfId="54"/>
+    <tableColumn id="3" xr3:uid="{041E9CBC-7CE4-48BB-A7AA-7F30F7569802}" name="mit / ohne Offset" dataDxfId="53"/>
+    <tableColumn id="4" xr3:uid="{7E07C587-1EB0-46B8-8F3E-3E35F9D0164D}" name="Anzahl Rechenknoten" dataDxfId="52"/>
+    <tableColumn id="5" xr3:uid="{D4DEF5B0-A627-47E8-8759-112E0628B432}" name="Populationsgröße" dataDxfId="51"/>
+    <tableColumn id="6" xr3:uid="{33BA195D-8889-4763-870A-82A2CAD42ED1}" name="(Start-) Rekombinationsrate" dataDxfId="50"/>
+    <tableColumn id="7" xr3:uid="{D42B36FD-F1B8-4765-B14B-0AB4CD534307}" name="Delta Rekombinationsrate" dataDxfId="49"/>
+    <tableColumn id="8" xr3:uid="{BF2EEC5F-7304-428F-BD91-0C65B3BEE72F}" name="Anzahl Elitisten" dataDxfId="48"/>
+    <tableColumn id="9" xr3:uid="{5570D174-D9C8-401C-BF23-66D36038F518}" name="Offset" dataDxfId="47"/>
+    <tableColumn id="10" xr3:uid="{53F23BD6-14B8-41B8-857A-3A139FD7C9A4}" name="Iterationen" dataDxfId="46"/>
+    <tableColumn id="11" xr3:uid="{16F8028F-1019-46E3-A47D-C03426554D87}" name="Notizen" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3262786E-EADB-4970-8DCB-0C3E2CA0491F}" name="Tabelle13" displayName="Tabelle13" ref="A1:L21" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3262786E-EADB-4970-8DCB-0C3E2CA0491F}" name="Tabelle13" displayName="Tabelle13" ref="A1:L21" totalsRowShown="0" headerRowDxfId="44" dataDxfId="42" headerRowBorderDxfId="43" tableBorderDxfId="41" totalsRowBorderDxfId="40">
   <autoFilter ref="A1:L21" xr:uid="{3262786E-EADB-4970-8DCB-0C3E2CA0491F}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{EBC23620-6299-4F9E-A03B-152D8E926588}" name="Rekombinationstyp" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{CE58E6EA-5E62-4C09-A41A-25E14FAF4683}" name="Typ Rekombinationsrate" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{BA2EBEAD-E4F6-4987-A4E4-1071392DCCA5}" name="mit / ohne Offset" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{D80D805A-F3FB-480D-B4C5-4B4895EEB25F}" name="Anzahl Rechenknoten" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{A9B0E371-630B-42B8-8C42-C5655A4B7427}" name="Populationsgröße" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{7D465FE8-FC65-4466-9518-38A3A9D9BCF4}" name="(Start-) Rekombinationsrate" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{4E443DEE-E707-4BA3-B361-077E8DABF672}" name="Delta Rekombinationsrate" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{DE16DA46-B7E3-4CA6-BD65-AD82812E3778}" name="Anzahl Elitisten" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{56ED5AAA-44A8-44EB-A016-F7592A40B9FE}" name="Offset" dataDxfId="17"/>
-    <tableColumn id="10" xr3:uid="{02B02A40-7CC6-460A-9FEA-54286618D688}" name="Iterationen" dataDxfId="16"/>
-    <tableColumn id="11" xr3:uid="{44D1ABA5-7523-42BC-8FF9-CC1C035DB5D4}" name="Fitness" dataDxfId="15"/>
-    <tableColumn id="12" xr3:uid="{8DB525A8-4B8A-476B-970A-75523C0137D6}" name="Notizen" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{EBC23620-6299-4F9E-A03B-152D8E926588}" name="Rekombinationstyp" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{CE58E6EA-5E62-4C09-A41A-25E14FAF4683}" name="Typ Rekombinationsrate" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{BA2EBEAD-E4F6-4987-A4E4-1071392DCCA5}" name="mit / ohne Offset" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{D80D805A-F3FB-480D-B4C5-4B4895EEB25F}" name="Anzahl Rechenknoten" dataDxfId="36"/>
+    <tableColumn id="5" xr3:uid="{A9B0E371-630B-42B8-8C42-C5655A4B7427}" name="Populationsgröße" dataDxfId="35"/>
+    <tableColumn id="6" xr3:uid="{7D465FE8-FC65-4466-9518-38A3A9D9BCF4}" name="(Start-) Rekombinationsrate" dataDxfId="34"/>
+    <tableColumn id="7" xr3:uid="{4E443DEE-E707-4BA3-B361-077E8DABF672}" name="Delta Rekombinationsrate" dataDxfId="33"/>
+    <tableColumn id="8" xr3:uid="{DE16DA46-B7E3-4CA6-BD65-AD82812E3778}" name="Anzahl Elitisten" dataDxfId="32"/>
+    <tableColumn id="9" xr3:uid="{56ED5AAA-44A8-44EB-A016-F7592A40B9FE}" name="Offset" dataDxfId="31"/>
+    <tableColumn id="10" xr3:uid="{02B02A40-7CC6-460A-9FEA-54286618D688}" name="Iterationen" dataDxfId="30"/>
+    <tableColumn id="11" xr3:uid="{44D1ABA5-7523-42BC-8FF9-CC1C035DB5D4}" name="Fitness" dataDxfId="29"/>
+    <tableColumn id="12" xr3:uid="{8DB525A8-4B8A-476B-970A-75523C0137D6}" name="Notizen" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{16E9E3FF-82F7-4D02-89F5-0EFEBB302DBC}" name="Tabelle14" displayName="Tabelle14" ref="A1:I20" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{16E9E3FF-82F7-4D02-89F5-0EFEBB302DBC}" name="Tabelle14" displayName="Tabelle14" ref="A1:I20" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26" tableBorderDxfId="24" totalsRowBorderDxfId="23">
   <autoFilter ref="A1:I20" xr:uid="{16E9E3FF-82F7-4D02-89F5-0EFEBB302DBC}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{E3061643-506C-4DF5-9519-25A5F354EE28}" name="Rekombinationstyp" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{1FD88150-3719-40E4-9930-3DAD021E5786}" name="Typ Rekombinationsrate" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{2947C2F6-045E-4DD9-834F-AD1EC2D305C1}" name="mit / ohne Offset" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{D1559373-156A-4445-926B-0BBB80142A0C}" name="Anzahl Rechenknoten" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{B3F81709-CC4C-4398-AAAF-ACC6C4B7DD92}" name="Populationsgröße" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{0455A311-9330-4D66-878D-DE22D808F49F}" name="(Start-) Rekombinationsrate" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{94BA1A90-5769-4BC9-90CB-E9F5241EEC52}" name="Delta Rekombinationsrate" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{6866B354-ACD0-490F-96F7-E4A2DEFB0D0F}" name="Anzahl Elitisten" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{514CBF92-64C9-4012-B295-3CB710414703}" name="Offset" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{E3061643-506C-4DF5-9519-25A5F354EE28}" name="Rekombinationstyp" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{1FD88150-3719-40E4-9930-3DAD021E5786}" name="Typ Rekombinationsrate" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{2947C2F6-045E-4DD9-834F-AD1EC2D305C1}" name="mit / ohne Offset" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{D1559373-156A-4445-926B-0BBB80142A0C}" name="Anzahl Rechenknoten" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{B3F81709-CC4C-4398-AAAF-ACC6C4B7DD92}" name="Populationsgröße" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{0455A311-9330-4D66-878D-DE22D808F49F}" name="(Start-) Rekombinationsrate" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{94BA1A90-5769-4BC9-90CB-E9F5241EEC52}" name="Delta Rekombinationsrate" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{6866B354-ACD0-490F-96F7-E4A2DEFB0D0F}" name="Anzahl Elitisten" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{514CBF92-64C9-4012-B295-3CB710414703}" name="Offset" dataDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CD4597CE-3872-4047-A550-B90A263C707E}" name="Tabelle145" displayName="Tabelle145" ref="A1:I20" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
+  <autoFilter ref="A1:I20" xr:uid="{CD4597CE-3872-4047-A550-B90A263C707E}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{0BB7C5C8-FFEB-4668-AF70-EAB37989D023}" name="Rekombinationstyp" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{C47DA794-2036-487F-9DD0-C73265E7354E}" name="Typ Rekombinationsrate" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{12CB1741-6318-48DE-AD6E-25557C5EC463}" name="mit / ohne Offset" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{A09FA44E-E89E-4CA2-9FA5-1AF5F648ACA4}" name="Anzahl Rechenknoten" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{23DBF58F-AA14-48C1-B4DF-2F1F75EADB43}" name="Populationsgröße" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{D96791C3-F52F-4204-B118-43E2DA6F7CA8}" name="(Start-) Rekombinationsrate" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{5EB4F068-87F6-45DC-8ED4-D3AA8219818D}" name="Delta Rekombinationsrate" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{A24E0D09-B4CA-4DC2-A7FA-E1ABD4751D2B}" name="Anzahl Elitisten" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{86526C6C-2BAE-4D80-8D1E-621E253EA342}" name="Offset" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3094,8 +3389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23A0EA66-8E87-4152-A235-1FC7EB76D9FD}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F5" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3600,4 +3895,516 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EFFC37E-59A8-4DB9-AEF9-46177000D81C}">
+  <dimension ref="A1:J22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="71.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="7">
+        <v>6000</v>
+      </c>
+      <c r="E2" s="7">
+        <v>48</v>
+      </c>
+      <c r="F2" s="14"/>
+      <c r="G2" s="7">
+        <v>0</v>
+      </c>
+      <c r="H2" s="7">
+        <v>8</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="7">
+        <v>6000</v>
+      </c>
+      <c r="E3" s="7">
+        <v>48</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5">
+        <v>0</v>
+      </c>
+      <c r="H3" s="7">
+        <v>8</v>
+      </c>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="7">
+        <v>6000</v>
+      </c>
+      <c r="E4" s="7">
+        <v>48</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="7">
+        <v>8</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="7">
+        <v>6000</v>
+      </c>
+      <c r="E5" s="7">
+        <v>48</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="7">
+        <v>8</v>
+      </c>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="7">
+        <v>6000</v>
+      </c>
+      <c r="E6" s="7">
+        <v>48</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5">
+        <v>0</v>
+      </c>
+      <c r="H6" s="7">
+        <v>8</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="7">
+        <v>6000</v>
+      </c>
+      <c r="E7" s="7">
+        <v>48</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5">
+        <v>0</v>
+      </c>
+      <c r="H7" s="7">
+        <v>8</v>
+      </c>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="9">
+        <v>2500</v>
+      </c>
+      <c r="E8" s="9">
+        <v>50</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9">
+        <v>0</v>
+      </c>
+      <c r="H8" s="7">
+        <v>8</v>
+      </c>
+      <c r="I8" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="9">
+        <v>2500</v>
+      </c>
+      <c r="E9" s="9">
+        <v>50</v>
+      </c>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9">
+        <v>0</v>
+      </c>
+      <c r="H9" s="7">
+        <v>8</v>
+      </c>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="9">
+        <v>2500</v>
+      </c>
+      <c r="E10" s="9">
+        <v>50</v>
+      </c>
+      <c r="F10" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="G10" s="9"/>
+      <c r="H10" s="7">
+        <v>8</v>
+      </c>
+      <c r="I10" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="9">
+        <v>2500</v>
+      </c>
+      <c r="E11" s="9">
+        <v>50</v>
+      </c>
+      <c r="F11" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="7">
+        <v>8</v>
+      </c>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="9">
+        <v>2500</v>
+      </c>
+      <c r="E12" s="9">
+        <v>50</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9">
+        <v>0</v>
+      </c>
+      <c r="H12" s="7">
+        <v>8</v>
+      </c>
+      <c r="I12" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="8"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="9">
+        <v>2500</v>
+      </c>
+      <c r="E13" s="9">
+        <v>50</v>
+      </c>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9">
+        <v>0</v>
+      </c>
+      <c r="H13" s="7">
+        <v>8</v>
+      </c>
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="5">
+        <v>3500</v>
+      </c>
+      <c r="E14" s="5">
+        <v>48</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5">
+        <v>0</v>
+      </c>
+      <c r="H14" s="9">
+        <v>2</v>
+      </c>
+      <c r="I14" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="5">
+        <v>3500</v>
+      </c>
+      <c r="E15" s="5">
+        <v>48</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5">
+        <v>0</v>
+      </c>
+      <c r="H15" s="9">
+        <v>2</v>
+      </c>
+      <c r="I15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="5">
+        <v>3500</v>
+      </c>
+      <c r="E16" s="5">
+        <v>48</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="9">
+        <v>2</v>
+      </c>
+      <c r="I16" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="5">
+        <v>3500</v>
+      </c>
+      <c r="E17" s="5">
+        <v>48</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="G17" s="5"/>
+      <c r="H17" s="9">
+        <v>2</v>
+      </c>
+      <c r="I17" s="5"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" s="4"/>
+      <c r="B18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="5">
+        <v>3500</v>
+      </c>
+      <c r="E18" s="5">
+        <v>48</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5">
+        <v>0</v>
+      </c>
+      <c r="H18" s="9">
+        <v>2</v>
+      </c>
+      <c r="I18" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="5">
+        <v>3500</v>
+      </c>
+      <c r="E19" s="5">
+        <v>48</v>
+      </c>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5">
+        <v>0</v>
+      </c>
+      <c r="H19" s="9">
+        <v>2</v>
+      </c>
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="12">
+        <v>5500</v>
+      </c>
+      <c r="E20" s="12">
+        <v>50</v>
+      </c>
+      <c r="F20" s="12">
+        <v>0</v>
+      </c>
+      <c r="G20" s="12">
+        <v>0</v>
+      </c>
+      <c r="H20" s="12">
+        <v>6</v>
+      </c>
+      <c r="I20" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J22" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
hpo analyse keijzer und parity
</commit_message>
<xml_diff>
--- a/julia-nix-slurm-env-main/HPOErgebnisse.xlsx
+++ b/julia-nix-slurm-env-main/HPOErgebnisse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\49160\Documents\Master\Masterarbeit\OC-MasterThesis\julia-nix-slurm-env-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7679A813-AF2E-4BB1-88A2-A532644B8371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1489912F-F00B-4029-8C4D-ECCFB7B42BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="5" xr2:uid="{FC45CD7E-7F2F-48B4-8C22-E79589995154}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FC45CD7E-7F2F-48B4-8C22-E79589995154}"/>
   </bookViews>
   <sheets>
     <sheet name="Parity" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="32">
   <si>
     <t>Konstant</t>
   </si>
@@ -123,6 +123,21 @@
   <si>
     <t>Bester Wert hat kein Offset! Zweitbesten nehmen! Werte Bester: [1950, 56, 0.8, 18, 0]</t>
   </si>
+  <si>
+    <t>Mittelwert alle</t>
+  </si>
+  <si>
+    <t>Mittelwert OnePoint</t>
+  </si>
+  <si>
+    <t>Mittelwert TwoPoint</t>
+  </si>
+  <si>
+    <t>Mittelwert Uniform</t>
+  </si>
+  <si>
+    <t>Mittelwert Offset</t>
+  </si>
 </sst>
 </file>
 
@@ -133,10 +148,16 @@
     <numFmt numFmtId="165" formatCode="0.00000000"/>
     <numFmt numFmtId="166" formatCode="0.000000000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -553,35 +574,35 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -2260,7 +2281,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{0CA0A5D1-7FC0-4490-A059-179BD9B0A707}" name="Tabelle14567" displayName="Tabelle14567" ref="A1:I20" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{0CA0A5D1-7FC0-4490-A059-179BD9B0A707}" name="Tabelle14567" displayName="Tabelle14567" ref="A1:I20" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
   <autoFilter ref="A1:I20" xr:uid="{0CA0A5D1-7FC0-4490-A059-179BD9B0A707}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{FF6D2C93-AC3B-4AF8-BEC6-0318F0452975}" name="Rekombinationstyp" dataDxfId="8"/>
@@ -2594,10 +2615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24624115-2EA4-43F4-B7C3-9E45AC575B2C}">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="D9" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3242,6 +3263,53 @@
         <v>54.915788831208843</v>
       </c>
     </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23">
+        <f>AVERAGE(Tabelle1[Anzahl Rechenknoten])</f>
+        <v>1305.2631578947369</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24">
+        <f>AVERAGE(D2:D7)</f>
+        <v>1441.6666666666667</v>
+      </c>
+      <c r="H24" t="s">
+        <v>31</v>
+      </c>
+      <c r="I24">
+        <f>AVERAGE(I3,I5,I7,I9,I11,I13,I15,I17,I19)</f>
+        <v>26.666666666666668</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C25" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25">
+        <f>AVERAGE(D8:D13)</f>
+        <v>1325</v>
+      </c>
+      <c r="I25">
+        <f>AVERAGE(I3,I5,I8,I9,I12,I13,I15,I17,I19)</f>
+        <v>21.111111111111111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26">
+        <f>AVERAGE(D14:D19)</f>
+        <v>1200</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -3252,10 +3320,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD7223BD-063A-4B3D-9902-0134A848554C}">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="E6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3967,7 +4035,55 @@
       <c r="K21" s="18"/>
       <c r="L21" s="18"/>
     </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24">
+        <f>AVERAGE(Tabelle1[Anzahl Rechenknoten])</f>
+        <v>1305.2631578947369</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25">
+        <f>AVERAGE(D2:D7)</f>
+        <v>1016.6666666666666</v>
+      </c>
+      <c r="H25" t="s">
+        <v>31</v>
+      </c>
+      <c r="I25">
+        <f>AVERAGE(I3,I5,I7,I9,I11,I13,I15,I17,I19)</f>
+        <v>153.33333333333334</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C26" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26">
+        <f>AVERAGE(D8:D13)</f>
+        <v>983.33333333333337</v>
+      </c>
+      <c r="I26">
+        <f>AVERAGE(I3,I6,I7,I10,I11,I15,I13,I17,I19)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27">
+        <f>AVERAGE(D14:D19)</f>
+        <v>1300</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -5515,7 +5631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5076A12-71FE-4894-A98D-480079E9D503}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>

</xml_diff>